<commit_message>
Updating ACC vs F1 results
</commit_message>
<xml_diff>
--- a/SVM/results_v2.xlsx
+++ b/SVM/results_v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t>Accuracy</t>
   </si>
@@ -169,6 +169,69 @@
   <si>
     <t>5 23
 22 360</t>
+  </si>
+  <si>
+    <t>4 22
+16 368</t>
+  </si>
+  <si>
+    <t>0.17299145299145297</t>
+  </si>
+  <si>
+    <t>5 21
+22 362</t>
+  </si>
+  <si>
+    <t>5 20
+20 365</t>
+  </si>
+  <si>
+    <t>0.26853146853146853</t>
+  </si>
+  <si>
+    <t>8 17
+23 362</t>
+  </si>
+  <si>
+    <t>5 13
+7 385</t>
+  </si>
+  <si>
+    <t>0.2631578947368421</t>
+  </si>
+  <si>
+    <t>5 13
+15 377</t>
+  </si>
+  <si>
+    <t>0 12
+7 391</t>
+  </si>
+  <si>
+    <t>0 12
+9 389</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0 10
+6 394</t>
+  </si>
+  <si>
+    <t>0 10
+3 397</t>
+  </si>
+  <si>
+    <t>0.05714285714285715</t>
+  </si>
+  <si>
+    <t>1 7
+8 394</t>
+  </si>
+  <si>
+    <t>1 7
+10 392</t>
   </si>
 </sst>
 </file>
@@ -306,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -315,7 +378,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -639,7 +701,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,7 +757,7 @@
       <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -704,7 +766,7 @@
       <c r="G3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>31</v>
       </c>
       <c r="I3" t="s">
@@ -718,7 +780,7 @@
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -727,7 +789,7 @@
       <c r="G4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>33</v>
       </c>
     </row>
@@ -738,7 +800,7 @@
       <c r="B5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>35</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -747,7 +809,7 @@
       <c r="G5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>37</v>
       </c>
     </row>
@@ -758,7 +820,7 @@
       <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>38</v>
       </c>
       <c r="F6" s="6" t="s">
@@ -767,7 +829,7 @@
       <c r="G6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -778,7 +840,7 @@
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F7" s="6" t="s">
@@ -787,105 +849,141 @@
       <c r="G7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="11" t="s">
+        <v>45</v>
+      </c>
       <c r="F8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="F9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="F10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G10" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="F11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G11" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="F12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="11" t="s">
+        <v>61</v>
+      </c>
       <c r="F13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
+      <c r="G13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="F14" s="9" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="F14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>